<commit_message>
Changed the script to include all the sheets, updated Readme.md
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,12 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6825001-332E-43B3-B8A7-000551468D93}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00C56C7-B9A7-4105-B8E3-E7AF018542C7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>watewet</t>
   </si>
@@ -361,10 +364,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49FB5BE-7406-4625-87B0-9123EDF93313}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,27 +430,121 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9BAEEE-6067-4B9D-A5BF-990F1CF9EADB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483F0950-4BFA-4F9D-9B41-0C987ABF6A33}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>